<commit_message>
update latex report and spreadsheet
</commit_message>
<xml_diff>
--- a/CSCI446_Project1_GraphColoring/Official Output Results/SizeDecisionsSpreadsheet.xlsx
+++ b/CSCI446_Project1_GraphColoring/Official Output Results/SizeDecisionsSpreadsheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Graph Size</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>BCP</t>
+  </si>
+  <si>
+    <t>AVERAGE DECISIONS MADE</t>
   </si>
 </sst>
 </file>
@@ -78,7 +81,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,12 +104,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -117,6 +129,9 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -401,7 +416,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,193 +429,172 @@
     <col min="6" max="6" width="16.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>10</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="5">
         <v>248.25</v>
       </c>
-      <c r="D2" s="5">
-        <v>350.8</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="E3" s="5">
         <v>73.75</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F3" s="5">
         <v>909</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1548.95</v>
-      </c>
-      <c r="D3" s="5">
-        <v>363.85</v>
-      </c>
-      <c r="E3" s="5">
-        <v>301.45</v>
-      </c>
-      <c r="F3" s="5">
-        <v>11924</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5">
-        <v>88013.1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>795.65</v>
+        <v>1548.95</v>
       </c>
       <c r="E4" s="5">
-        <v>12271.3</v>
+        <v>301.45</v>
       </c>
       <c r="F4" s="5">
-        <v>91857</v>
+        <v>11924</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5">
-        <v>26853.95</v>
-      </c>
-      <c r="D5" s="5">
-        <v>-1</v>
+        <v>88013.1</v>
       </c>
       <c r="E5" s="5">
-        <v>3568.9</v>
+        <v>12271.3</v>
       </c>
       <c r="F5" s="5">
-        <v>676264</v>
+        <v>91857</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5">
-        <v>321947.95</v>
-      </c>
-      <c r="D6" s="5">
-        <v>-1</v>
+        <v>26853.95</v>
       </c>
       <c r="E6" s="5">
-        <v>31755.4</v>
+        <v>3568.9</v>
       </c>
       <c r="F6" s="5">
-        <v>2564917</v>
+        <v>676264</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C7" s="5">
-        <v>1902743.35</v>
-      </c>
-      <c r="D7" s="5">
-        <v>648.20000000000005</v>
+        <v>321947.95</v>
       </c>
       <c r="E7" s="5">
-        <v>136544.85</v>
+        <v>31755.4</v>
       </c>
       <c r="F7" s="5">
-        <v>1712152</v>
+        <v>2564917</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C8" s="5">
-        <v>702684.1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>-1</v>
+        <v>1902743.35</v>
       </c>
       <c r="E8" s="5">
-        <v>56496.2</v>
+        <v>136544.85</v>
       </c>
       <c r="F8" s="5">
-        <v>3510198</v>
+        <v>1712152</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C9" s="5">
-        <v>50391248.850000001</v>
-      </c>
-      <c r="D9" s="5">
-        <v>-1</v>
+        <v>702684.1</v>
       </c>
       <c r="E9" s="5">
-        <v>3137781.9</v>
+        <v>56496.2</v>
       </c>
       <c r="F9" s="5">
-        <v>4588425</v>
+        <v>3510198</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C10" s="5">
-        <v>-54884585.25</v>
-      </c>
-      <c r="D10" s="5">
-        <v>-1</v>
+        <v>50391248.850000001</v>
       </c>
       <c r="E10" s="5">
-        <v>8626512.0500000007</v>
+        <v>3137781.9</v>
       </c>
       <c r="F10" s="5">
-        <v>4634637</v>
+        <v>4588425</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-54884585.25</v>
+      </c>
+      <c r="E11" s="5">
+        <v>8626512.0500000007</v>
+      </c>
+      <c r="F11" s="5">
+        <v>4634637</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>100</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <v>72250484.75</v>
       </c>
-      <c r="D11" s="5">
-        <v>-1</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="E12" s="5">
         <v>3807202.45</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F12" s="5">
         <v>8181442</v>
       </c>
     </row>
@@ -641,6 +635,9 @@
       <c r="B26" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>